<commit_message>
Minor Test Data Update
</commit_message>
<xml_diff>
--- a/Test Excels/FMR_Crawler_Test_Excel.xlsx
+++ b/Test Excels/FMR_Crawler_Test_Excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SectionM8 Business Documents\SectionM8 Fall 2025 Demo\SectionM8-Demo-Fall2025\Test Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F40ECFD3-BD1B-47C0-AD40-AE67EAC22C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70013DB-D363-455E-80E9-0281669102A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FMR_Crawler_Test" sheetId="1" r:id="rId1"/>
@@ -133,16 +133,16 @@
     <t>ETL_001</t>
   </si>
   <si>
-    <t>Aston</t>
-  </si>
-  <si>
     <t>New Jersey</t>
   </si>
   <si>
     <t>NJ</t>
   </si>
   <si>
-    <t>Camden</t>
+    <t>Delaware County</t>
+  </si>
+  <si>
+    <t>Camden County</t>
   </si>
 </sst>
 </file>
@@ -485,15 +485,15 @@
   <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W8" sqref="A1:W8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="18" max="18" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -564,7 +564,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2025</v>
       </c>
@@ -617,7 +617,7 @@
         <v>1</v>
       </c>
       <c r="R2">
-        <v>84500</v>
+        <v>85000</v>
       </c>
       <c r="S2" t="s">
         <v>32</v>
@@ -635,7 +635,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2025</v>
       </c>
@@ -706,7 +706,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2025</v>
       </c>
@@ -759,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="R4">
-        <v>84000</v>
+        <v>85000</v>
       </c>
       <c r="S4" t="s">
         <v>32</v>
@@ -777,7 +777,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2025</v>
       </c>
@@ -788,7 +788,7 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <v>42091</v>
@@ -848,7 +848,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2025</v>
       </c>
@@ -859,7 +859,7 @@
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E6">
         <v>42091</v>
@@ -901,7 +901,7 @@
         <v>1</v>
       </c>
       <c r="R6">
-        <v>96000</v>
+        <v>80000</v>
       </c>
       <c r="S6" t="s">
         <v>32</v>
@@ -919,7 +919,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2025</v>
       </c>
@@ -930,7 +930,7 @@
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E7">
         <v>42091</v>
@@ -972,7 +972,7 @@
         <v>1</v>
       </c>
       <c r="R7">
-        <v>100000</v>
+        <v>80000</v>
       </c>
       <c r="S7" t="s">
         <v>32</v>
@@ -990,15 +990,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2025</v>
       </c>
       <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
         <v>38</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
       </c>
       <c r="D8" t="s">
         <v>40</v>
@@ -1043,7 +1043,7 @@
         <v>1</v>
       </c>
       <c r="R8">
-        <v>130000</v>
+        <v>67000</v>
       </c>
       <c r="S8" t="s">
         <v>32</v>

</xml_diff>